<commit_message>
Framework Exceptions are implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testlogin.xlsx
+++ b/src/test/resources/excel/testlogin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>testname</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>To Check wheather the test is executed</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>loginTest</t>
   </si>
 </sst>
 </file>
@@ -428,14 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
     <col min="3" max="3" width="13.453125" customWidth="1"/>
     <col min="4" max="4" width="20.1796875" customWidth="1"/>
     <col min="5" max="5" width="16.81640625" customWidth="1"/>
@@ -462,8 +469,8 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -496,8 +503,8 @@
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -516,10 +523,10 @@
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -531,7 +538,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -541,6 +548,23 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -555,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TC Appoinment History created
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testlogin.xlsx
+++ b/src/test/resources/excel/testlogin.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -30,9 +30,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
@@ -81,17 +78,38 @@
     <t>To Check wheather the test is executed</t>
   </si>
   <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>loginTest</t>
+  </si>
+  <si>
+    <t>expectedvalue</t>
+  </si>
+  <si>
+    <t>loginWithInvalidCredentials</t>
+  </si>
+  <si>
+    <t>Login failed! Please ensure the username and password are valid.</t>
+  </si>
+  <si>
+    <t>testdata</t>
+  </si>
+  <si>
+    <t>verifyUserCanBookAppoinment</t>
+  </si>
+  <si>
+    <t>Hongkong CURA Healthcare Center,Medicaid,02/12/2024,cough and fever</t>
+  </si>
+  <si>
+    <t>Please be informed that your appointment has been booked as following:</t>
+  </si>
+  <si>
+    <t>verifyAppoinmentHistory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +123,19 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +162,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -139,6 +170,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -434,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -445,10 +478,11 @@
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="3" max="3" width="13.453125" customWidth="1"/>
     <col min="4" max="4" width="20.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="55.90625" customWidth="1"/>
+    <col min="6" max="6" width="67.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,110 +495,191 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -572,6 +687,7 @@
     <hyperlink ref="D6" r:id="rId1" display="Admin@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -594,27 +710,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -625,13 +741,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>2</v>

</xml_diff>